<commit_message>
update the availability if teh check-out date is lower than current date
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,106 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kikea\PycharmProjects\cp317\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DECECD-3BB0-4D62-A629-AE0392CF490A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Rooms" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Rooms" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t>Room number</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>View</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>Check-in</t>
-  </si>
-  <si>
-    <t>Check-out</t>
-  </si>
-  <si>
-    <t>Client Name</t>
-  </si>
-  <si>
-    <t>Client Phone</t>
-  </si>
-  <si>
-    <t>Amendities</t>
-  </si>
-  <si>
-    <t>022</t>
-  </si>
-  <si>
-    <t>Double Room</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>Monument</t>
-  </si>
-  <si>
-    <t>077</t>
-  </si>
-  <si>
-    <t>Deluxe Room</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -128,24 +64,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -465,91 +461,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" customWidth="1"/>
+    <col width="18.44140625" customWidth="1" min="1" max="1"/>
+    <col width="17.6640625" customWidth="1" min="2" max="2"/>
+    <col width="16.109375" customWidth="1" min="3" max="3"/>
+    <col width="16.5546875" customWidth="1" min="4" max="4"/>
+    <col width="13.88671875" customWidth="1" min="5" max="5"/>
+    <col width="15.88671875" customWidth="1" min="6" max="7"/>
+    <col width="17.88671875" customWidth="1" min="8" max="8"/>
+    <col width="19.5546875" customWidth="1" min="9" max="9"/>
+    <col width="32" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
+    <row r="1" ht="20.4" customHeight="1" thickBot="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Room number</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>View</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Check-in</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Check-out</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Client Name</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Client Phone</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Amendities</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
+    <row r="2" ht="15" customHeight="1" thickTop="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>022</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Double Room</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Monument</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>077</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Deluxe Room</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>333</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Suite</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Garden</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n"/>
+      <c r="G4" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -558,12 +627,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Testing button to showcase when a checkout date has passed
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -466,10 +466,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -614,11 +614,115 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>2024-12-06</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>2024-12-11</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Carlos Alcoba</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>263262662</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Pool, Dinner, Room Service</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>044</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Single Room</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>170</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="F4" s="2" t="n"/>
-      <c r="G4" s="2" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>028</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Suite</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>340</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>050</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Double Room</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Monument</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>